<commit_message>
Commit by Farheen: Implement the address field in Location master, Implement the Tax value field in Tax master and Bind the grid view for Inward QC sorting successfully.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Company.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Company.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC634386-160D-44A9-85B8-C5F88CCB6F76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12789BE4-EBC4-473B-9D27-34F8A8B58C9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{6F127CB0-B9FF-4DB5-986B-8D945220DED4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TM_0001</t>
   </si>
@@ -67,24 +67,6 @@
   </si>
   <si>
     <t>IsBlackListed</t>
-  </si>
-  <si>
-    <t>DEF</t>
-  </si>
-  <si>
-    <t>Buyer</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>afd</t>
-  </si>
-  <si>
-    <t>fd</t>
-  </si>
-  <si>
-    <t>ds</t>
   </si>
 </sst>
 </file>
@@ -154,7 +136,57 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -515,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DE3A76-C534-483E-A884-AABFD63B277F}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,52 +622,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>9854213615</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H3">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -645,16 +642,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter valid value!" sqref="I2:J1048576" xr:uid="{153C1E98-C7E7-48BA-8B19-0D047E1057A2}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter valid mobile no" sqref="E2:E3" xr:uid="{F0C8D21F-F9C0-48E8-BF50-F1A7DC2891D3}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter valid mobile no" sqref="E2" xr:uid="{F0C8D21F-F9C0-48E8-BF50-F1A7DC2891D3}">
       <formula1>0</formula1>
       <formula2>13</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{39A55AE4-4EC7-4592-8EC9-BB2728CBF3ED}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{338F58C4-73AE-4622-A77F-8E59568C2F49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit by Farheen: Resolve the bug InVan-35, and did validation in Item master module.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Company.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Company.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eroff\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12789BE4-EBC4-473B-9D27-34F8A8B58C9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB39CD7-4ACF-418B-86C2-4C9B5938D92B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{6F127CB0-B9FF-4DB5-986B-8D945220DED4}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>TM_0001</t>
-  </si>
-  <si>
     <t>CompanyName</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>EmailId</t>
   </si>
   <si>
-    <t>ABC company name</t>
-  </si>
-  <si>
     <t>abc@gmail.com</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>IsBlackListed</t>
+  </si>
+  <si>
+    <t>DEF company</t>
+  </si>
+  <si>
+    <t>Sunny</t>
   </si>
 </sst>
 </file>
@@ -136,67 +136,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -550,7 +490,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,48 +509,48 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>9854213615</v>
@@ -619,18 +559,18 @@
         <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>